<commit_message>
Add luận giải về cung Quan
</commit_message>
<xml_diff>
--- a/LuanQuanLoc.xlsx
+++ b/LuanQuanLoc.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AEDD66A-4D40-4B11-B63A-6A780E7FD38A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DE90F9AF-D931-497A-9D2C-285F42EB765A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2940" yWindow="2940" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Cơ Nguyệt Đồng Lương</t>
   </si>
@@ -43,6 +43,48 @@
   </si>
   <si>
     <t>Đại vận chủ về công việc gặp rất nhiều vấn đề xấu.</t>
+  </si>
+  <si>
+    <t>Quan Lộc có Thiên Lương thủ tọa tại Tý</t>
+  </si>
+  <si>
+    <t>Quan Lộc có Thiên Lương thủ tọa tại Hợi</t>
+  </si>
+  <si>
+    <t>Công việc nào cũng rất thích nhưng nhanh chán.</t>
+  </si>
+  <si>
+    <t>Hay thay đổi công việc.</t>
+  </si>
+  <si>
+    <t>Công việc có tính lưu động di chuyển.</t>
+  </si>
+  <si>
+    <t>Nên làm công việc có tính lưu động như du lịch, báo chí, hoặc lưu diễn...</t>
+  </si>
+  <si>
+    <t>Quan Lộc có Thiên Đồng Thiên Lương đồng cung</t>
+  </si>
+  <si>
+    <t>Công việc liên quan đến y dược, chính trị, sư phạm.</t>
+  </si>
+  <si>
+    <t>Đều có danh tiếng trong ngành y dược, sư phạm.</t>
+  </si>
+  <si>
+    <t>Quan Lộc có Tử Vi Thiên Tướng đồng cung"</t>
+  </si>
+  <si>
+    <t>Công việc liên quan đến quân đội, cảnh sát. Có tiền đồ phát triển liên quan đến quân sự, quốc phòng.</t>
+  </si>
+  <si>
+    <t>Có tài lãnh binh, điều hành, điều khiển, lãnh đạo, chỉ đạo.</t>
+  </si>
+  <si>
+    <t>Quan Lộc có Tham Lang Tử Vi đồng cung</t>
+  </si>
+  <si>
+    <t>Công việc bình thường, nếu công việc có nhiều thành công rực rỡ dễ dính vào tai họa ẩn nấp</t>
   </si>
 </sst>
 </file>
@@ -360,15 +402,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -379,17 +421,81 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>4</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>9</v>
+      </c>
+      <c r="D4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B5" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D5" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B8" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
giai thich hoan thien version 2
</commit_message>
<xml_diff>
--- a/LuanQuanLoc.xlsx
+++ b/LuanQuanLoc.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App_Tuvi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6690074A-53EB-452B-8C1C-5367B3E74A50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A70B6057-4C0D-46A1-AF05-83ABB326860F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3877" uniqueCount="2161">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3901" uniqueCount="2185">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -6543,6 +6543,78 @@
   </si>
   <si>
     <t>Công danh trắc trở. Lúc thiếu thời khó được xứng ý toại lòng, vì có tài nhưng bất đắc chí, về già mới có chút hư danh</t>
+  </si>
+  <si>
+    <t>Làm thầy thuốc có danh tiếng.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Làm thầy giáo, viết báo. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mở nhà in, làm tiểu công nghệ, hay buôn bán khá giả. </t>
+  </si>
+  <si>
+    <t>Làm thợ rất khéo léo</t>
+  </si>
+  <si>
+    <t>Chuyên ca vũ nhạc rất nổi tiếng.</t>
+  </si>
+  <si>
+    <t>Làm thợ may, thợ thêu</t>
+  </si>
+  <si>
+    <t>Làm thợ vẽ, hay họa sĩ</t>
+  </si>
+  <si>
+    <t>Làm công chức nhỏ thấp, làm quản lý, tổ trưởng.</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương Tướng Ấn Long Phượng Phù</t>
+  </si>
+  <si>
+    <t>Làm thầy bói số cao tay</t>
+  </si>
+  <si>
+    <t>Làm thầy bối số</t>
+  </si>
+  <si>
+    <t>Thích xem bói toán, tâm linh</t>
+  </si>
+  <si>
+    <t>Làm thầy hòa thượng</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương Tả Hữu Quang Quý Quan Phúc hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương Tả Hữu Khoa Quyền Khôi Việt Xương Khúc Tấu hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương Tả Hữu Xương Khúc hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Tử Phủ Vũ Tướng Tả Hữu Long Phượng Hình Riêu hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Cơ Hồng Riêu Đào Tấu hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Cơ Hồng Tấu hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Sát Phá Liêm Tham Hồng Đào Tấu Long Phượng hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Cơ Nguyệt Đồng Lương Tả Hữu Xương Khúc Thai Cáo hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Sát Phá Liêm Tham Tả Hữu Quyền Lộc Nhật Nguyệt hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Đồng Long Phượng Hình Riêu Hồng Đào hội chiếu tại Quan Lộc</t>
+  </si>
+  <si>
+    <t>Thiên Tướng Quan Phù Tả Hữu Tướng Ấn hội chiếu tại Quan Lộc</t>
   </si>
 </sst>
 </file>
@@ -6593,28 +6665,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
+  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -6890,10 +6941,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G1936"/>
+  <dimension ref="A2:G1947"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1927" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B1935" sqref="B1935"/>
+    <sheetView tabSelected="1" topLeftCell="A1933" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="C1944" sqref="C1944"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -9365,7 +9416,7 @@
         <v>335</v>
       </c>
     </row>
-    <row r="309" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="309" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A309" s="1" t="s">
         <v>336</v>
       </c>
@@ -11325,7 +11376,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="554" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="554" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A554" s="1" t="s">
         <v>579</v>
       </c>
@@ -15029,7 +15080,7 @@
         <v>1041</v>
       </c>
     </row>
-    <row r="1017" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1017" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1017" s="1" t="s">
         <v>1042</v>
       </c>
@@ -16061,7 +16112,7 @@
         <v>1975</v>
       </c>
     </row>
-    <row r="1146" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="1146" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1146" s="1" t="s">
         <v>1171</v>
       </c>
@@ -16069,7 +16120,7 @@
         <v>1976</v>
       </c>
     </row>
-    <row r="1147" spans="1:2" ht="90" x14ac:dyDescent="0.25">
+    <row r="1147" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1147" s="1" t="s">
         <v>1172</v>
       </c>
@@ -22458,11 +22509,105 @@
       <c r="F1935" s="1"/>
       <c r="G1935" s="1"/>
     </row>
-    <row r="1936" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1936" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1936" s="1" t="s">
+        <v>2174</v>
+      </c>
+      <c r="B1936" s="1" t="s">
+        <v>2161</v>
+      </c>
       <c r="C1936" s="1"/>
       <c r="D1936" s="1"/>
       <c r="E1936" s="1"/>
       <c r="F1936" s="3"/>
+    </row>
+    <row r="1937" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1937" s="1" t="s">
+        <v>2175</v>
+      </c>
+      <c r="B1937" s="1" t="s">
+        <v>2162</v>
+      </c>
+    </row>
+    <row r="1938" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1938" s="1" t="s">
+        <v>2176</v>
+      </c>
+      <c r="B1938" s="1" t="s">
+        <v>2163</v>
+      </c>
+    </row>
+    <row r="1939" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1939" s="1" t="s">
+        <v>2177</v>
+      </c>
+      <c r="B1939" s="1" t="s">
+        <v>2164</v>
+      </c>
+    </row>
+    <row r="1940" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1940" s="1" t="s">
+        <v>2178</v>
+      </c>
+      <c r="B1940" s="1" t="s">
+        <v>2165</v>
+      </c>
+    </row>
+    <row r="1941" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1941" s="1" t="s">
+        <v>2179</v>
+      </c>
+      <c r="B1941" s="1" t="s">
+        <v>2166</v>
+      </c>
+    </row>
+    <row r="1942" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1942" s="1" t="s">
+        <v>2180</v>
+      </c>
+      <c r="B1942" t="s">
+        <v>2167</v>
+      </c>
+    </row>
+    <row r="1943" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1943" s="1" t="s">
+        <v>2181</v>
+      </c>
+      <c r="B1943" s="1" t="s">
+        <v>2168</v>
+      </c>
+    </row>
+    <row r="1944" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1944" s="1" t="s">
+        <v>2169</v>
+      </c>
+      <c r="B1944" s="1" t="s">
+        <v>2170</v>
+      </c>
+    </row>
+    <row r="1945" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1945" s="1" t="s">
+        <v>2182</v>
+      </c>
+      <c r="B1945" s="1" t="s">
+        <v>2171</v>
+      </c>
+    </row>
+    <row r="1946" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1946" s="1" t="s">
+        <v>2183</v>
+      </c>
+      <c r="B1946" s="1" t="s">
+        <v>2172</v>
+      </c>
+    </row>
+    <row r="1947" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1947" s="1" t="s">
+        <v>2184</v>
+      </c>
+      <c r="B1947" s="1" t="s">
+        <v>2173</v>
+      </c>
     </row>
   </sheetData>
   <autoFilter ref="A2:E1935" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>

</xml_diff>